<commit_message>
edit search and statics controller and web and excel and production view
</commit_message>
<xml_diff>
--- a/public/files/excel/date_production.xlsx
+++ b/public/files/excel/date_production.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
     <t>رقم التوظيف</t>
   </si>
@@ -23,10 +23,22 @@
     <t>عدد الأمتار</t>
   </si>
   <si>
+    <t>المجموعة</t>
+  </si>
+  <si>
+    <t>الوردية</t>
+  </si>
+  <si>
     <t>تاريخ الإنتاج</t>
   </si>
   <si>
-    <t>2021-02-27</t>
+    <t>الثالثة</t>
+  </si>
+  <si>
+    <t>صباحية</t>
+  </si>
+  <si>
+    <t>2021-03-01</t>
   </si>
 </sst>
 </file>
@@ -365,7 +377,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -373,7 +385,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -383,49 +395,28 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2">
-        <v>109</v>
+        <v>185</v>
       </c>
       <c r="B2">
-        <v>700</v>
+        <v>5000</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>109</v>
-      </c>
-      <c r="B3">
-        <v>500</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>661</v>
-      </c>
-      <c r="B4">
-        <v>500</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>661</v>
-      </c>
-      <c r="B5">
-        <v>1000</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>